<commit_message>
fix locator on become partner page
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/BecomePartnerPage.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/BecomePartnerPage.xlsx
@@ -135,12 +135,6 @@
     <t>#Partner_Interest__c</t>
   </si>
   <si>
-    <t>#mktoCheckbox_139660_0</t>
-  </si>
-  <si>
-    <t>#LblmktoCheckbox_139660_0</t>
-  </si>
-  <si>
     <t>button.mktoButton[type='submit']</t>
   </si>
   <si>
@@ -247,6 +241,12 @@
   </si>
   <si>
     <t>BecomePartnerPage_Modal_Label_ViewPrivacyPolicy</t>
+  </si>
+  <si>
+    <t>#mktoCheckbox_144792_0</t>
+  </si>
+  <si>
+    <t>#LblmktoCheckbox_144792_0</t>
   </si>
 </sst>
 </file>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -813,7 +813,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -824,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -832,10 +832,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -843,10 +843,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -854,10 +854,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -865,10 +865,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -876,10 +876,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -887,10 +887,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -898,10 +898,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -909,10 +909,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -920,10 +920,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -931,10 +931,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -942,10 +942,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -953,10 +953,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -964,10 +964,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -975,10 +975,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -986,10 +986,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -997,10 +997,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1008,10 +1008,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1019,10 +1019,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Locators for Become partner page
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/BecomePartnerPage.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/BecomePartnerPage.xlsx
@@ -135,12 +135,6 @@
     <t>#Partner_Interest__c</t>
   </si>
   <si>
-    <t>#mktoCheckbox_139660_0</t>
-  </si>
-  <si>
-    <t>#LblmktoCheckbox_139660_0</t>
-  </si>
-  <si>
     <t>button.mktoButton[type='submit']</t>
   </si>
   <si>
@@ -243,10 +237,16 @@
     <t>BecomePartnerPage_BrandLogo_ImageLink</t>
   </si>
   <si>
+    <t>BecomePartnerPage_Modal_Label_ViewPrivacyPolicy</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Privacy Policy')]/parent::span/ancestor::div/input</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Privacy Policy')]/parent::span/ancestor::label</t>
+  </si>
+  <si>
     <t>//a[contains(text(),'Privacy Policy')]/parent::span/parent::div</t>
-  </si>
-  <si>
-    <t>BecomePartnerPage_Modal_Label_ViewPrivacyPolicy</t>
   </si>
 </sst>
 </file>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,10 +623,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -634,10 +634,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -645,10 +645,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -656,10 +656,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -667,10 +667,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -700,10 +700,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -711,10 +711,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -722,10 +722,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -733,10 +733,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -744,10 +744,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -755,10 +755,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -766,10 +766,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -777,10 +777,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -788,10 +788,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -799,10 +799,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -810,10 +810,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -821,10 +821,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -832,10 +832,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -843,10 +843,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -854,10 +854,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -865,10 +865,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -876,10 +876,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -887,10 +887,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -898,10 +898,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -909,10 +909,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -920,10 +920,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -931,10 +931,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -942,10 +942,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -953,10 +953,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -964,10 +964,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -975,10 +975,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -986,10 +986,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -997,10 +997,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1008,10 +1008,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1019,13 +1019,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B2:C38">
+    <sortCondition ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>